<commit_message>
foi adicionado o Hash, Unittest e o Smtpblib
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -1,37 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="5001191-57.2022.8.13.0334" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="0000047-02.2023.8.13.0334" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="5000141-59.2023.8.13.0334" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -50,21 +49,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -330,13 +388,478 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Número Processo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Data de Distribuição</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Movimentações</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>5001191-57.2022.8.13.0334</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>5001191-57.2022.8.13.0334</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>16/03/2023 17:29:52 - Arquivado Definitivamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>16/03/2023 13:15:16 - Juntada de certidão de baixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>15/03/2023 17:06:09 - Proferido despacho de mero expediente</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>14/03/2023 13:00:08 - Expedição de Certidão.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>08/03/2023 12:55:15 - Conclusos para Juiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>16/02/2023 13:22:13 - Juntada de Petição de informações prestadas</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>26/01/2023 17:30:18 - Expedição de Certidão.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>13/01/2023 16:21:02 - Expedição de Certidão.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>05/10/2022 12:58:11 - Juntada de Petição de manifestação da promotoria</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>04/10/2022 12:28:43 - Expedição de comunicação via sistema.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>03/10/2022 18:50:29 - Outras Decisões</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>01/08/2022 12:37:50 - Conclusos para Juiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>29/07/2022 15:37:04 - Juntada de Petição de manifestação da promotoria</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>29/07/2022 11:02:49 - Remetidos os Autos (Órgão Julgador de Plantão) para Vara Única da Comarca de Itapagipe</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>29/07/2022 10:07:39 - Declarada incompetência</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Número Processo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Data de Distribuição</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Movimentações</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0000047-02.2023.8.13.0334</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0000047-02.2023.8.13.0334</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>17/08/2023 16:02:02 - Juntada de Mandado</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>17/08/2023 15:45:50 - Juntada de Mandado</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>14/08/2023 12:09:32 - Juntada de Ofício</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>12/08/2023 14:52:08 - Juntada de Outros documentos</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>10/08/2023 17:57:20 - Juntada de Outros documentos</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>10/08/2023 13:31:10 - Expedição de Mandado.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>10/08/2023 13:05:30 - Juntada de Ofício</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>09/08/2023 18:19:07 - Expedição de Carta precatória.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>07/07/2023 15:27:43 - Juntada de Petição de petição</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>07/07/2023 15:20:04 - Juntada de Petição de petição</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>16/06/2023 00:52:23 - Decorrido prazo de GUILHERME DE CAMPOS MARCONATO em 15/06/2023 23:59.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>25/05/2023 17:54:50 - Expedição de comunicação via sistema.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>04/05/2023 09:57:30 - Juntada de Sentença</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>18/04/2023 00:55:59 - Decorrido prazo de GUILHERME DE CAMPOS MARCONATO em 17/04/2023 23:59.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>31/03/2023 08:56:18 - Juntada de Petição de manifestação da promotoria</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Número Processo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Data de Distribuição</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Movimentações</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>5000141-59.2023.8.13.0334</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>5000141-59.2023.8.13.0334</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>22/05/2023 13:42:13 - Arquivado Definitivamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>19/05/2023 17:12:45 - Juntada de certidão de trânsito em julgado - jesp</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>04/04/2023 01:12:19 - Decorrido prazo de GUILHERME DE CAMPOS MARCONATO em 03/04/2023 23:59.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>09/03/2023 15:03:15 - Juntada de Petição de manifestação</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>03/03/2023 12:51:52 - Expedição de comunicação via sistema.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>03/03/2023 12:51:52 - Expedição de comunicação via sistema.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>03/03/2023 12:51:32 - Audiência Conciliação cancelada para 19/04/2023 14:00 Juizado Especial da Comarca de Itapagipe</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>02/03/2023 18:30:58 - Extinta a execução ou o cumprimento da sentença</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>02/03/2023 18:30:58 - Homologada a Transação</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>01/03/2023 10:57:30 - Juntada de Petição de manifestação</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>28/02/2023 17:42:06 - Conclusos para decisão</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>27/02/2023 14:27:58 - Juntada de Petição de manifestação</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>31/01/2023 17:24:58 - Expedição de carta via correio.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>31/01/2023 16:59:33 - Expedição de Certidão de Triagem.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>27/01/2023 15:58:47 - Audiência Conciliação designada para 19/04/2023 14:00 Juizado Especial da Comarca de Itapagipe</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>